<commit_message>
Contact Page TC added
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9335" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" r:id="rId1"/>
     <sheet name="Credentials" sheetId="2" r:id="rId2"/>
+    <sheet name="NewContact" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>title</t>
   </si>
@@ -75,6 +76,27 @@
   </si>
   <si>
     <t>Abcd@123456</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>allowCalls</t>
+  </si>
+  <si>
+    <t>Prashant</t>
+  </si>
+  <si>
+    <t>Hule</t>
+  </si>
+  <si>
+    <t>Mastek</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -82,10 +104,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -112,6 +134,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -120,6 +150,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -127,47 +164,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -182,21 +186,45 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,16 +246,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -235,21 +263,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -264,7 +286,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,19 +466,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,164 +476,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -464,13 +486,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -490,6 +534,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -505,15 +558,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -525,15 +569,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -555,164 +590,168 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="7" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1035,64 +1074,64 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelRow="3" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1107,8 +1146,8 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1118,18 +1157,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1140,4 +1179,60 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6" outlineLevelRow="1" outlineLevelCol="4"/>
+  <cols>
+    <col min="2" max="2" width="10.6" customWidth="1"/>
+    <col min="3" max="4" width="10.3" customWidth="1"/>
+    <col min="5" max="5" width="10.7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>